<commit_message>
fix wrong parent for dpv:hasScale properties
- fixes (source, RDF, HTML) dpv:hasScale where child properties instead
  had dpv:Scale as the parent
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/purpose_processing.xlsx
+++ b/documentation-generator/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="726">
   <si>
     <t>Term</t>
   </si>
@@ -2393,6 +2393,9 @@
   </si>
   <si>
     <t>Indicates the volume of data</t>
+  </si>
+  <si>
+    <t>dpv:hasScale</t>
   </si>
   <si>
     <t>https://www.w3.org/2022/06/22-dpvcg-minutes.html</t>
@@ -42303,7 +42306,7 @@
         <v>649</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>646</v>
+        <v>718</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -42320,7 +42323,7 @@
         <v>81</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -42338,13 +42341,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
@@ -42353,7 +42356,7 @@
         <v>666</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>646</v>
+        <v>718</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -42370,7 +42373,7 @@
         <v>81</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -42388,13 +42391,13 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
@@ -42403,7 +42406,7 @@
         <v>682</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>646</v>
+        <v>718</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -42420,7 +42423,7 @@
         <v>81</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>

</xml_diff>

<commit_message>
adds diagrams to spec/primer; fixes concept error
- adds diagrams Processing Context, Context, location, rights, risk
- fixes error in ProcessingContext where EvaluationScoring was not
  declared as the parent for EvaluationOfIndividuals and
  ScoringOfIndividuals
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/purpose_processing.xlsx
+++ b/documentation-generator/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="748">
   <si>
     <t>Term</t>
   </si>
@@ -2075,6 +2075,9 @@
   </si>
   <si>
     <t>Processing that involves evaluation of individuals</t>
+  </si>
+  <si>
+    <t>dpv:EvaluationScoring</t>
   </si>
   <si>
     <t>ScoringOfIndividuals</t>
@@ -30871,7 +30874,7 @@
         <v>611</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>532</v>
+        <v>612</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>34</v>
@@ -30886,9 +30889,11 @@
       <c r="K33" s="9">
         <v>44856.0</v>
       </c>
-      <c r="L33" s="8"/>
+      <c r="L33" s="9">
+        <v>44895.0</v>
+      </c>
       <c r="M33" s="5" t="s">
-        <v>22</v>
+        <v>294</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>81</v>
@@ -30907,21 +30912,19 @@
       <c r="Z33" s="8"/>
       <c r="AA33" s="8"/>
       <c r="AB33" s="8"/>
-      <c r="AC33" s="8"/>
-      <c r="AD33" s="8"/>
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>612</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>613</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>614</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>532</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>34</v>
@@ -30936,9 +30939,11 @@
       <c r="K34" s="9">
         <v>44856.0</v>
       </c>
-      <c r="L34" s="8"/>
+      <c r="L34" s="9">
+        <v>44895.0</v>
+      </c>
       <c r="M34" s="5" t="s">
-        <v>22</v>
+        <v>294</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>81</v>
@@ -30957,18 +30962,16 @@
       <c r="Z34" s="8"/>
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
-      <c r="AC34" s="8"/>
-      <c r="AD34" s="8"/>
     </row>
     <row r="35">
       <c r="A35" s="109" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B35" s="110" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>532</v>
@@ -31010,13 +31013,13 @@
     </row>
     <row r="37">
       <c r="A37" s="109" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B37" s="110" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C37" s="112" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>532</v>
@@ -31062,13 +31065,13 @@
     </row>
     <row r="39">
       <c r="A39" s="65" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B39" s="58" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>532</v>
@@ -31112,13 +31115,13 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>503</v>
@@ -31162,16 +31165,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>34</v>
@@ -31212,16 +31215,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>34</v>
@@ -31262,13 +31265,13 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>503</v>
@@ -31312,13 +31315,13 @@
     </row>
     <row r="44">
       <c r="A44" s="109" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B44" s="110" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C44" s="112" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>532</v>
@@ -36167,13 +36170,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>532</v>
@@ -36185,7 +36188,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="90" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="9">
@@ -36196,7 +36199,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>99</v>
@@ -36229,16 +36232,16 @@
     </row>
     <row r="4">
       <c r="A4" s="65" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>34</v>
@@ -36256,7 +36259,7 @@
         <v>22</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>99</v>
@@ -36277,16 +36280,16 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
@@ -36325,16 +36328,16 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>655</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>653</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>654</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>652</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>18</v>
@@ -36373,16 +36376,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
@@ -36400,7 +36403,7 @@
         <v>22</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>99</v>
@@ -36421,16 +36424,16 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
@@ -36469,16 +36472,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C9" s="94" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>18</v>
@@ -36517,16 +36520,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
@@ -36577,16 +36580,16 @@
     </row>
     <row r="12">
       <c r="A12" s="65" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>34</v>
@@ -36604,7 +36607,7 @@
         <v>22</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="O12" s="10" t="s">
         <v>99</v>
@@ -36625,16 +36628,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C13" s="95" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
@@ -36673,16 +36676,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>678</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>676</v>
-      </c>
-      <c r="B14" s="58" t="s">
-        <v>677</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>678</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>675</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>18</v>
@@ -36721,16 +36724,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>18</v>
@@ -36748,7 +36751,7 @@
         <v>22</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="O15" s="10" t="s">
         <v>99</v>
@@ -36769,16 +36772,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>18</v>
@@ -36817,16 +36820,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>18</v>
@@ -36865,16 +36868,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -36925,16 +36928,16 @@
     </row>
     <row r="20">
       <c r="A20" s="65" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>34</v>
@@ -36952,7 +36955,7 @@
         <v>22</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="O20" s="10" t="s">
         <v>99</v>
@@ -36973,16 +36976,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
@@ -37021,16 +37024,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>698</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>699</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>700</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>697</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>18</v>
@@ -37069,16 +37072,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -37117,16 +37120,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
@@ -37165,16 +37168,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -37213,16 +37216,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -37231,7 +37234,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="90" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="9">
@@ -37263,16 +37266,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -37281,7 +37284,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="90" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="9">
@@ -37324,16 +37327,16 @@
     </row>
     <row r="29">
       <c r="A29" s="65" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>34</v>
@@ -37342,7 +37345,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="116" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="9">
@@ -37372,16 +37375,16 @@
     </row>
     <row r="30">
       <c r="A30" s="118" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B30" s="119" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C30" s="120" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D30" s="121" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E30" s="121" t="s">
         <v>18</v>
@@ -37390,7 +37393,7 @@
       <c r="G30" s="122"/>
       <c r="H30" s="122"/>
       <c r="I30" s="116" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="J30" s="123" t="s">
         <v>378</v>
@@ -37428,16 +37431,16 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D31" s="109" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>18</v>
@@ -37474,16 +37477,16 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D32" s="109" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>18</v>
@@ -42304,19 +42307,19 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>360</v>
@@ -42354,22 +42357,22 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -42386,7 +42389,7 @@
         <v>81</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -42404,22 +42407,22 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -42436,7 +42439,7 @@
         <v>81</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -42454,22 +42457,22 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -42486,7 +42489,7 @@
         <v>81</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>

</xml_diff>